<commit_message>
Updated BIS 3 display names according to v6 changes
</commit_message>
<xml_diff>
--- a/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Document types v5.xlsx
+++ b/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Document types v5.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="125">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -186,9 +186,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:billing:3.0::2.1</t>
   </si>
   <si>
-    <t>PEPPOL BIS Billing V3</t>
-  </si>
-  <si>
     <t>DHSC Customized Ordering profile V1</t>
   </si>
   <si>
@@ -394,6 +391,15 @@
   </si>
   <si>
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.2::D16B</t>
+  </si>
+  <si>
+    <t>PEPPOL BIS Billing UBL Invoice V3</t>
+  </si>
+  <si>
+    <t>PEPPOL BIS Billing UBL CreditNote V3</t>
+  </si>
+  <si>
+    <t>PEPPOL BIS Billing CII Invoice V3</t>
   </si>
 </sst>
 </file>
@@ -894,7 +900,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -911,13 +917,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
@@ -934,7 +940,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -955,7 +961,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -976,7 +982,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
@@ -997,7 +1003,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
@@ -1018,7 +1024,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -1039,7 +1045,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -1060,7 +1066,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>33</v>
@@ -1078,7 +1084,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1099,10 +1105,10 @@
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>29</v>
@@ -1115,7 +1121,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="29">
@@ -1123,10 +1129,10 @@
         <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="8">
         <v>3</v>
@@ -1141,7 +1147,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
@@ -1162,7 +1168,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
@@ -1180,7 +1186,7 @@
         <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
@@ -1201,7 +1207,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
@@ -1222,7 +1228,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
@@ -1243,7 +1249,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>36</v>
@@ -1261,7 +1267,7 @@
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>37</v>
@@ -1279,7 +1285,7 @@
         <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1297,7 +1303,7 @@
         <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1315,7 +1321,7 @@
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -1333,7 +1339,7 @@
         <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1351,7 +1357,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1369,7 +1375,7 @@
         <v>38</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -1387,7 +1393,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>23</v>
@@ -1408,7 +1414,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>25</v>
@@ -1426,7 +1432,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>43</v>
@@ -1444,7 +1450,7 @@
         <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>44</v>
@@ -1459,7 +1465,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="29">
@@ -1467,10 +1473,10 @@
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="8">
         <v>3</v>
@@ -1485,7 +1491,7 @@
         <v>45</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>47</v>
@@ -1503,7 +1509,7 @@
         <v>46</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>48</v>
@@ -1518,10 +1524,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="4" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>51</v>
@@ -1536,10 +1542,10 @@
     </row>
     <row r="33" spans="1:6" ht="29">
       <c r="A33" s="4" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>52</v>
@@ -1554,13 +1560,13 @@
     </row>
     <row r="34" spans="1:6" ht="43.5">
       <c r="A34" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="8">
         <v>3</v>
@@ -1572,13 +1578,13 @@
     </row>
     <row r="35" spans="1:6" ht="43.5">
       <c r="A35" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="8">
         <v>3</v>
@@ -1590,13 +1596,13 @@
     </row>
     <row r="36" spans="1:6" ht="29">
       <c r="A36" s="4" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36" s="6">
         <v>3</v>
@@ -1608,13 +1614,13 @@
     </row>
     <row r="37" spans="1:6" ht="29">
       <c r="A37" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" s="6">
         <v>3</v>
@@ -1626,13 +1632,13 @@
     </row>
     <row r="38" spans="1:6" ht="29">
       <c r="A38" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D38" s="6">
         <v>3</v>
@@ -1644,13 +1650,13 @@
     </row>
     <row r="39" spans="1:6" ht="29">
       <c r="A39" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" s="6">
         <v>3</v>
@@ -1662,13 +1668,13 @@
     </row>
     <row r="40" spans="1:6" ht="29">
       <c r="A40" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D40" s="6">
         <v>3</v>
@@ -1680,13 +1686,13 @@
     </row>
     <row r="41" spans="1:6" ht="29">
       <c r="A41" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" s="6">
         <v>3</v>
@@ -1698,13 +1704,13 @@
     </row>
     <row r="42" spans="1:6" ht="29">
       <c r="A42" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42" s="6">
         <v>3</v>
@@ -1716,13 +1722,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="D43" s="10">
         <v>3</v>
@@ -1736,13 +1742,13 @@
     </row>
     <row r="44" spans="1:6" ht="29">
       <c r="A44" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="D44" s="10">
         <v>3</v>
@@ -1756,13 +1762,13 @@
     </row>
     <row r="45" spans="1:6" ht="29">
       <c r="A45" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45" s="10">
         <v>3</v>
@@ -1776,13 +1782,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" s="10">
         <v>3</v>
@@ -1794,13 +1800,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D47" s="10">
         <v>3</v>
@@ -1812,13 +1818,13 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D48" s="10">
         <v>3</v>
@@ -1830,13 +1836,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D49" s="10">
         <v>3</v>
@@ -1848,13 +1854,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D50" s="6">
         <v>4</v>
@@ -1866,13 +1872,13 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D51" s="10">
         <v>4</v>
@@ -1884,13 +1890,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D52" s="10">
         <v>4</v>
@@ -1902,13 +1908,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D53" s="10">
         <v>4</v>
@@ -1920,13 +1926,13 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D54" s="10">
         <v>4</v>
@@ -1938,13 +1944,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D55" s="10">
         <v>4</v>
@@ -1956,13 +1962,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D56" s="10">
         <v>4</v>
@@ -1974,13 +1980,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D57" s="10">
         <v>4</v>
@@ -1992,13 +1998,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D58" s="10">
         <v>4</v>
@@ -2010,13 +2016,13 @@
     </row>
     <row r="59" spans="1:5" ht="29">
       <c r="A59" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D59" s="10">
         <v>4</v>
@@ -2028,13 +2034,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="D60" s="10">
         <v>4</v>
@@ -2046,13 +2052,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="D61" s="10">
         <v>4</v>
@@ -2064,13 +2070,13 @@
     </row>
     <row r="62" spans="1:5" ht="29">
       <c r="A62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D62" s="10">
         <v>4</v>
@@ -2082,13 +2088,13 @@
     </row>
     <row r="63" spans="1:5" ht="29">
       <c r="A63" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="D63" s="10">
         <v>4</v>
@@ -2100,13 +2106,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D64" s="6">
         <v>5</v>
@@ -2118,13 +2124,13 @@
     </row>
     <row r="65" spans="1:5" ht="29">
       <c r="A65" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D65" s="6">
         <v>5</v>
@@ -2136,13 +2142,13 @@
     </row>
     <row r="66" spans="1:5" ht="29">
       <c r="A66" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D66" s="6">
         <v>5</v>

</xml_diff>

<commit_message>
Used document type profile code from V6 draft
</commit_message>
<xml_diff>
--- a/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Document types v5.xlsx
+++ b/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Document types v5.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="136">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -111,9 +111,6 @@
     <t>PEPPOL Invoice profile V2</t>
   </si>
   <si>
-    <t>PEPPOL Catalogue profile V1</t>
-  </si>
-  <si>
     <t>1.2.0</t>
   </si>
   <si>
@@ -129,30 +126,18 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:Catalogue-2::Catalogue##urn:www.cenbii.eu:transaction:biitrns019:ver2.0:extended:urn:www.peppol.eu:bis:peppol1a:ver4.0::2.1</t>
   </si>
   <si>
-    <t>PEPPOL Billing profile V1</t>
-  </si>
-  <si>
-    <t>PEPPOL Billing profile V2</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:www.cenbii.eu:transaction:biitrns010:ver2.0:extended:urn:www.peppol.eu:bis:peppol5a:ver2.0::2.1</t>
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:www.cenbii.eu:transaction:biitrns014:ver2.0:extended:urn:www.peppol.eu:bis:peppol5a:ver2.0::2.1</t>
   </si>
   <si>
-    <t>PEPPOL Procurement profile V1</t>
-  </si>
-  <si>
     <t>EHF Invoice V1</t>
   </si>
   <si>
     <t>Standalone Credit Note according to EHF V1</t>
   </si>
   <si>
-    <t>PEPPOL Ordering profile V1</t>
-  </si>
-  <si>
     <t>PEPPOL Catalogue profile V4</t>
   </si>
   <si>
@@ -186,12 +171,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:billing:3.0::2.1</t>
   </si>
   <si>
-    <t>DHSC Customized Ordering profile V1</t>
-  </si>
-  <si>
-    <t>DHSC Customized  Ordering profile V1</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:www.cenbii.eu:transaction:biitrns001:ver2.0:extended:urn:www.peppol.eu:bis:peppol28a:ver1.0:extended:urn:fdc:peppol-authority.co.uk:spec:ordering:ver1.0::2.1</t>
   </si>
   <si>
@@ -207,15 +186,6 @@
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:billing:3.0::D16B</t>
   </si>
   <si>
-    <t>Procurement procedure subscription V1</t>
-  </si>
-  <si>
-    <t>Procurement document access V1</t>
-  </si>
-  <si>
-    <t>Tender Submission V1</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ExpressionOfInterestRequest-2::ExpressionOfInterestRequest##urn:www.cenbii.eu:transaction:biitrdm081:ver3.0:extended:urn:fdc:peppol.eu:2017:pracc:t001:ver1.0::2.2</t>
   </si>
   <si>
@@ -249,12 +219,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.1::2.1</t>
   </si>
   <si>
-    <t>XRechnung Invoice V1.1</t>
-  </si>
-  <si>
-    <t>XRechnung CreditNote V1.1</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.1::2.1</t>
   </si>
   <si>
@@ -400,6 +364,75 @@
   </si>
   <si>
     <t>PEPPOL BIS Billing CII Invoice V3</t>
+  </si>
+  <si>
+    <t>PEPPOL Catalogue profile Catalogue V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Catalogue profile ApplicationResponse V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Billing profile Invoice V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Billing profile CreditNote V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Billing profile Invoice V2</t>
+  </si>
+  <si>
+    <t>PEPPOL Billing profile CreditNote V2</t>
+  </si>
+  <si>
+    <t>PEPPOL Procurement profile Order V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Procurement profile OrderResponseSimple V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Procurement profile Invoice V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Procurement profile CreditNote V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Ordering profile Order V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Ordering profile OrderResponse V1</t>
+  </si>
+  <si>
+    <t>DHSC Customized Ordering profile Order V1</t>
+  </si>
+  <si>
+    <t>DHSC Customized  Ordering profile OrderResponse V1</t>
+  </si>
+  <si>
+    <t>Procurement procedure subscription Request V1</t>
+  </si>
+  <si>
+    <t>Procurement procedure subscription Response V1</t>
+  </si>
+  <si>
+    <t>Procurement document access TenderStatusRequest V1</t>
+  </si>
+  <si>
+    <t>Procurement document access CallForTenders V1</t>
+  </si>
+  <si>
+    <t>Tender Submission TenderReceipt V1</t>
+  </si>
+  <si>
+    <t>Tender Submission Tender V1</t>
+  </si>
+  <si>
+    <t>XRechnung UBL Invoice V1.1</t>
+  </si>
+  <si>
+    <t>XRechnung UBL CreditNote V1.1</t>
+  </si>
+  <si>
+    <t>XRechnung CII Invoice V1.1</t>
   </si>
 </sst>
 </file>
@@ -465,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -493,6 +526,16 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -899,8 +942,8 @@
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -917,30 +960,30 @@
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="29">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -957,11 +1000,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="29">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -978,11 +1021,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="29">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
@@ -999,11 +1042,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="29">
-      <c r="A5" s="4" t="s">
-        <v>28</v>
+      <c r="A5" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
@@ -1020,11 +1063,11 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="29">
-      <c r="A6" s="4" t="s">
-        <v>28</v>
+      <c r="A6" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -1041,11 +1084,11 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29">
-      <c r="A7" s="4" t="s">
-        <v>28</v>
+      <c r="A7" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -1062,29 +1105,29 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29">
-      <c r="A8" s="4" t="s">
-        <v>42</v>
+      <c r="A8" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29">
+      <c r="A9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="29">
-      <c r="A9" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1101,17 +1144,17 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="29">
-      <c r="A10" s="2" t="s">
-        <v>31</v>
+      <c r="A10" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="10" t="b">
         <f>TRUE</f>
@@ -1121,18 +1164,18 @@
         <v>3</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="29">
-      <c r="A11" s="2" t="s">
-        <v>31</v>
+      <c r="A11" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D11" s="8">
         <v>3</v>
@@ -1143,11 +1186,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="29">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
@@ -1164,17 +1207,17 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="6" t="b">
         <f>FALSE</f>
@@ -1182,11 +1225,11 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29">
-      <c r="A14" s="2" t="s">
-        <v>34</v>
+      <c r="A14" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
@@ -1203,11 +1246,11 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29">
-      <c r="A15" s="2" t="s">
-        <v>34</v>
+      <c r="A15" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
@@ -1224,11 +1267,11 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="29">
-      <c r="A16" s="2" t="s">
-        <v>34</v>
+      <c r="A16" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
@@ -1245,17 +1288,17 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="29">
-      <c r="A17" s="2" t="s">
-        <v>35</v>
+      <c r="A17" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="6" t="b">
         <f>FALSE</f>
@@ -1263,17 +1306,17 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="29">
-      <c r="A18" s="2" t="s">
-        <v>35</v>
+      <c r="A18" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="6" t="b">
         <f>FALSE</f>
@@ -1281,11 +1324,11 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="29">
-      <c r="A19" s="4" t="s">
-        <v>38</v>
+      <c r="A19" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1299,11 +1342,11 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="29">
-      <c r="A20" s="4" t="s">
-        <v>38</v>
+      <c r="A20" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1317,11 +1360,11 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="29">
-      <c r="A21" s="4" t="s">
-        <v>38</v>
+      <c r="A21" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -1335,11 +1378,11 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="29">
-      <c r="A22" s="4" t="s">
-        <v>38</v>
+      <c r="A22" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1353,11 +1396,11 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="29">
-      <c r="A23" s="4" t="s">
-        <v>38</v>
+      <c r="A23" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1371,11 +1414,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="29">
-      <c r="A24" s="4" t="s">
-        <v>38</v>
+      <c r="A24" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -1389,11 +1432,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="29">
-      <c r="A25" s="4" t="s">
-        <v>39</v>
+      <c r="A25" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>23</v>
@@ -1410,11 +1453,11 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="43.5">
-      <c r="A26" s="4" t="s">
-        <v>40</v>
+      <c r="A26" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>25</v>
@@ -1428,17 +1471,17 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="29">
-      <c r="A27" s="4" t="s">
-        <v>41</v>
+      <c r="A27" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E27" s="6" t="b">
         <f>FALSE</f>
@@ -1446,17 +1489,17 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="29">
-      <c r="A28" s="4" t="s">
-        <v>41</v>
+      <c r="A28" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" s="6" t="b">
         <v>1</v>
@@ -1465,18 +1508,18 @@
         <v>3</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="29">
-      <c r="A29" s="4" t="s">
-        <v>41</v>
+      <c r="A29" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D29" s="8">
         <v>3</v>
@@ -1487,17 +1530,17 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="29">
-      <c r="A30" s="4" t="s">
-        <v>45</v>
+      <c r="A30" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="6" t="b">
         <f>FALSE</f>
@@ -1505,32 +1548,32 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="29">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="D32" s="6">
         <v>2</v>
@@ -1541,14 +1584,14 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="29">
-      <c r="A33" s="4" t="s">
-        <v>123</v>
+      <c r="A33" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D33" s="6">
         <v>2</v>
@@ -1559,14 +1602,14 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5">
-      <c r="A34" s="4" t="s">
-        <v>53</v>
+      <c r="A34" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D34" s="8">
         <v>3</v>
@@ -1577,14 +1620,14 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5">
-      <c r="A35" s="4" t="s">
-        <v>54</v>
+      <c r="A35" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D35" s="8">
         <v>3</v>
@@ -1595,14 +1638,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="29">
-      <c r="A36" s="4" t="s">
-        <v>124</v>
+      <c r="A36" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D36" s="6">
         <v>3</v>
@@ -1613,14 +1656,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="29">
-      <c r="A37" s="10" t="s">
-        <v>60</v>
+      <c r="A37" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D37" s="6">
         <v>3</v>
@@ -1631,14 +1674,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29">
-      <c r="A38" s="10" t="s">
-        <v>60</v>
+      <c r="A38" s="14" t="s">
+        <v>128</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D38" s="6">
         <v>3</v>
@@ -1649,14 +1692,14 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29">
-      <c r="A39" s="10" t="s">
-        <v>61</v>
+      <c r="A39" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D39" s="6">
         <v>3</v>
@@ -1667,14 +1710,14 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29">
-      <c r="A40" s="10" t="s">
-        <v>61</v>
+      <c r="A40" s="14" t="s">
+        <v>130</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D40" s="6">
         <v>3</v>
@@ -1685,14 +1728,14 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29">
-      <c r="A41" s="10" t="s">
-        <v>62</v>
+      <c r="A41" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D41" s="6">
         <v>3</v>
@@ -1703,14 +1746,14 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29">
-      <c r="A42" s="10" t="s">
-        <v>62</v>
+      <c r="A42" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D42" s="6">
         <v>3</v>
@@ -1721,14 +1764,14 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="4" t="s">
-        <v>74</v>
+      <c r="A43" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D43" s="10">
         <v>3</v>
@@ -1741,14 +1784,14 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29">
-      <c r="A44" s="4" t="s">
-        <v>75</v>
+      <c r="A44" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D44" s="10">
         <v>3</v>
@@ -1761,14 +1804,14 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="29">
-      <c r="A45" s="4" t="s">
-        <v>74</v>
+      <c r="A45" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D45" s="10">
         <v>3</v>
@@ -1781,14 +1824,14 @@
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="4" t="s">
-        <v>79</v>
+      <c r="A46" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D46" s="10">
         <v>3</v>
@@ -1799,14 +1842,14 @@
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="4" t="s">
-        <v>80</v>
+      <c r="A47" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D47" s="10">
         <v>3</v>
@@ -1817,14 +1860,14 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="4" t="s">
-        <v>81</v>
+      <c r="A48" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D48" s="10">
         <v>3</v>
@@ -1835,14 +1878,14 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="4" t="s">
-        <v>82</v>
+      <c r="A49" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D49" s="10">
         <v>3</v>
@@ -1853,14 +1896,14 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="4" t="s">
-        <v>89</v>
+      <c r="A50" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D50" s="6">
         <v>4</v>
@@ -1871,14 +1914,14 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="4" t="s">
-        <v>99</v>
+      <c r="A51" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D51" s="10">
         <v>4</v>
@@ -1889,14 +1932,14 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="4" t="s">
-        <v>100</v>
+      <c r="A52" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D52" s="10">
         <v>4</v>
@@ -1907,14 +1950,14 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="4" t="s">
-        <v>101</v>
+      <c r="A53" s="13" t="s">
+        <v>89</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D53" s="10">
         <v>4</v>
@@ -1925,14 +1968,14 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="4" t="s">
-        <v>102</v>
+      <c r="A54" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D54" s="10">
         <v>4</v>
@@ -1943,14 +1986,14 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="4" t="s">
-        <v>103</v>
+      <c r="A55" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D55" s="10">
         <v>4</v>
@@ -1961,14 +2004,14 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="4" t="s">
-        <v>104</v>
+      <c r="A56" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D56" s="10">
         <v>4</v>
@@ -1979,14 +2022,14 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="4" t="s">
-        <v>105</v>
+      <c r="A57" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D57" s="10">
         <v>4</v>
@@ -1997,14 +2040,14 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="4" t="s">
-        <v>106</v>
+      <c r="A58" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D58" s="10">
         <v>4</v>
@@ -2015,14 +2058,14 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="29">
-      <c r="A59" s="4" t="s">
-        <v>107</v>
+      <c r="A59" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D59" s="10">
         <v>4</v>
@@ -2033,14 +2076,14 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="4" t="s">
-        <v>108</v>
+      <c r="A60" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D60" s="10">
         <v>4</v>
@@ -2051,14 +2094,14 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="4" t="s">
-        <v>110</v>
+      <c r="A61" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D61" s="10">
         <v>4</v>
@@ -2069,14 +2112,14 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="29">
-      <c r="A62" t="s">
-        <v>112</v>
+      <c r="A62" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D62" s="10">
         <v>4</v>
@@ -2087,14 +2130,14 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="29">
-      <c r="A63" s="4" t="s">
-        <v>113</v>
+      <c r="A63" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D63" s="10">
         <v>4</v>
@@ -2105,14 +2148,14 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="4" t="s">
-        <v>116</v>
+      <c r="A64" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D64" s="6">
         <v>5</v>
@@ -2123,14 +2166,14 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="29">
-      <c r="A65" s="4" t="s">
-        <v>117</v>
+      <c r="A65" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D65" s="6">
         <v>5</v>
@@ -2141,14 +2184,14 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="29">
-      <c r="A66" s="4" t="s">
-        <v>118</v>
+      <c r="A66" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D66" s="6">
         <v>5</v>

</xml_diff>